<commit_message>
Updating metadata for example datasets.
</commit_message>
<xml_diff>
--- a/example_data/DAKO/example_metadata_2.xlsx
+++ b/example_data/DAKO/example_metadata_2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="158">
   <si>
     <t xml:space="preserve">Original_Column</t>
   </si>
@@ -124,7 +124,10 @@
     <t xml:space="preserve">dark phase start</t>
   </si>
   <si>
-    <t xml:space="preserve">General</t>
+    <t xml:space="preserve">mouse_straing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C57BL/6N</t>
   </si>
   <si>
     <t xml:space="preserve">Title</t>
@@ -574,13 +577,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -602,8 +609,8 @@
   </sheetPr>
   <dimension ref="A1:X24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R17" activeCellId="0" sqref="R17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -723,865 +730,868 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="B6" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="N13" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="O13" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P13" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="Q13" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="R13" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="S13" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="T13" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="U13" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="V13" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="W13" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="X13" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="N14" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="O14" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="P14" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Q14" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="R14" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="S14" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="T14" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="U14" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="V14" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="W14" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="X14" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C15" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="D15" s="0" t="s">
-        <v>71</v>
-      </c>
       <c r="E15" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="F15" s="0" t="s">
-        <v>71</v>
-      </c>
       <c r="G15" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="H15" s="0" t="s">
-        <v>71</v>
-      </c>
       <c r="I15" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="J15" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="J15" s="0" t="s">
-        <v>71</v>
-      </c>
       <c r="K15" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="L15" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="L15" s="0" t="s">
-        <v>71</v>
-      </c>
       <c r="M15" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="N15" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="O15" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="O15" s="0" t="s">
-        <v>71</v>
-      </c>
       <c r="P15" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q15" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="Q15" s="0" t="s">
-        <v>71</v>
-      </c>
       <c r="R15" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="S15" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="T15" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="S15" s="0" t="s">
+      <c r="U15" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="V15" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="W15" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="T15" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="U15" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="V15" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="W15" s="0" t="s">
-        <v>71</v>
-      </c>
       <c r="X15" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N16" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="O16" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="P16" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="Q16" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="R16" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="S16" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="T16" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="U16" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="V16" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="W16" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="X16" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M17" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N17" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="O17" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="P17" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="Q17" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="R17" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="S17" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="T17" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="U17" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="V17" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="W17" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="X17" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C18" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="L18" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="M18" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="N18" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="O18" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="P18" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q18" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="R18" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="S18" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="T18" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="U18" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="V18" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="W18" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="X18" s="0" t="s">
         <v>81</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="K18" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="L18" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="M18" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="N18" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="O18" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="P18" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q18" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="R18" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="S18" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="T18" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="U18" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="V18" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="W18" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="X18" s="0" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K19" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="L19" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="M19" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="N19" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="O19" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="P19" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q19" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="R19" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="S19" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="T19" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="U19" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="V19" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="W19" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="B19" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="I19" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="J19" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="K19" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="L19" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="M19" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="N19" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="O19" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="P19" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q19" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="R19" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="S19" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="T19" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="U19" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="V19" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="W19" s="0" t="s">
-        <v>98</v>
-      </c>
       <c r="X19" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C20" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="I20" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="K20" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="L20" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="M20" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="N20" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="O20" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="P20" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q20" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="R20" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="S20" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="D20" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="I20" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="J20" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="K20" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="L20" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="M20" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="N20" s="0" t="s">
+      <c r="T20" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="O20" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="P20" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q20" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="R20" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="S20" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="T20" s="0" t="s">
-        <v>121</v>
-      </c>
       <c r="U20" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="V20" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="W20" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="X20" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="K21" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="L21" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="M21" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="N21" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="O21" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="P21" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q21" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="R21" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="S21" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="T21" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="U21" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="V21" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="W21" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="X21" s="0" t="s">
         <v>131</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="G21" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="H21" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="J21" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="K21" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="L21" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="M21" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="N21" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="O21" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="P21" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q21" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="R21" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="S21" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="T21" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="U21" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="V21" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="W21" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="X21" s="0" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="M22" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="N22" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="O22" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="P22" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q22" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="R22" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="S22" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="T22" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="O22" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="P22" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="Q22" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="R22" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="S22" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="T22" s="0" t="s">
-        <v>144</v>
-      </c>
       <c r="U22" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="V22" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="W22" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="X22" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="I23" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="K23" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="L23" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="M23" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="N23" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="O23" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="P23" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q23" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="R23" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="S23" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="T23" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="U23" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="V23" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="W23" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="X23" s="0" t="s">
         <v>155</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="G23" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="J23" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="K23" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="L23" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="M23" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="N23" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="O23" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="P23" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="Q23" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="R23" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="S23" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="T23" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="U23" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="V23" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="W23" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="X23" s="0" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>